<commit_message>
Dodanie obsługi skrzyżowań i cyfr w nazwach ulic
</commit_message>
<xml_diff>
--- a/docs/Wyniki zapytań.xlsx
+++ b/docs/Wyniki zapytań.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="727">
   <si>
     <t>Wawerska (Olszowa - kier. Rycerska)</t>
   </si>
@@ -2189,12 +2189,6 @@
     <t>Błąd w OSM - ulice Samorządowa i Konarskiego nie łączą się</t>
   </si>
   <si>
-    <t>Błąd w OSM - Rondo Reymonta i Żeromskiego nie należy do żadnej z ulic</t>
-  </si>
-  <si>
-    <t>Błąd w OSM - Rondo Andriollego i Matejki nie należy do żadnej z ulic</t>
-  </si>
-  <si>
     <t>Andriollego (Hoża - Powstańców Warszawy)</t>
   </si>
   <si>
@@ -2211,9 +2205,6 @@
   </si>
   <si>
     <t>Plac Wolności to nie ulica</t>
-  </si>
-  <si>
-    <t>Rondo androillego i pułaskiego nie należy do żadnej z ulic</t>
   </si>
 </sst>
 </file>
@@ -2566,8 +2557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C715"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2721,12 +2712,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>721</v>
+      <c r="B22" s="2" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2795,12 +2786,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>721</v>
+      <c r="B32" s="2" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2811,17 +2802,17 @@
         <v>717</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>722</v>
+      <c r="B34" s="2" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>717</v>
@@ -2848,7 +2839,7 @@
         <v>35</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2856,7 +2847,7 @@
         <v>36</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2864,7 +2855,7 @@
         <v>37</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2872,7 +2863,7 @@
         <v>38</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2880,7 +2871,7 @@
         <v>39</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2909,7 +2900,7 @@
         <v>43</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2922,7 +2913,7 @@
         <v>45</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2965,36 +2956,57 @@
       <c r="A55" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="B55" s="2" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="56" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="B56" s="2" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="57" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="B57" s="2" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="58" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B58" s="2" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="59" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="B59" s="2" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="60" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="B61" s="2" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -3011,7 +3023,7 @@
         <v>60</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3019,7 +3031,7 @@
         <v>61</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3027,48 +3039,60 @@
         <v>62</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>63</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    </row>
+    <row r="68" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>729</v>
+      <c r="B68" s="2" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="69" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="B69" s="2" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="B70" s="2" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="B71" s="2" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="B72" s="2" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>69</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>